<commit_message>
Test written. commiting before the first run
</commit_message>
<xml_diff>
--- a/input/dataInput.xlsx
+++ b/input/dataInput.xlsx
@@ -4,15 +4,27 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="15045" windowHeight="6405"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="124519"/>
+  <oleSize ref="A1:G10"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>SearchKey</t>
+  </si>
+  <si>
+    <t>iPhone</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -342,12 +354,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
After ruuning the testclass several times there seems to to a problem in fetching data from the excel and setting it to the excel sheet.
</commit_message>
<xml_diff>
--- a/input/dataInput.xlsx
+++ b/input/dataInput.xlsx
@@ -4,15 +4,15 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="15045" windowHeight="6405"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="11190" windowHeight="3750"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="data" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:G10"/>
+  <oleSize ref="A1:A2"/>
 </workbook>
 </file>
 
@@ -357,7 +357,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
setting data to xl feature is not working.Rest of the test is working fine
</commit_message>
<xml_diff>
--- a/input/dataInput.xlsx
+++ b/input/dataInput.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="11190" windowHeight="3750"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="15765" windowHeight="6405"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <t>SearchKey</t>
   </si>
   <si>
-    <t>iPhone</t>
+    <t>IPHONE</t>
   </si>
 </sst>
 </file>
@@ -357,7 +357,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>